<commit_message>
# Conclusions 18 - Learning rate 0.005 - Results - still too fast - accuracy bad: product .98 - Time is better 1.5 minutes vs. 3-3.5 minutes ### Conclusions going forward: - Go back to much lower learning rates - try 0.002 - twice as much as default
</commit_message>
<xml_diff>
--- a/output/18_learn_rate_0.005/best.xlsx
+++ b/output/18_learn_rate_0.005/best.xlsx
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.005</v>
+        <v>0.0001</v>
       </c>
       <c r="D2" t="n">
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F2" t="n">
         <v>200</v>
@@ -501,40 +501,40 @@
         <v>100</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0001</v>
+        <v>0.005</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L2" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9926999807357788</v>
       </c>
       <c r="M2" t="n">
-        <v>0.933899998664856</v>
+        <v>0.9824000000953674</v>
       </c>
       <c r="N2" t="n">
-        <v>113.91</v>
+        <v>87.73999999999999</v>
       </c>
       <c r="O2" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0113</v>
       </c>
       <c r="P2" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0112</v>
       </c>
       <c r="Q2" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="R2" t="n">
-        <v>5.6955</v>
+        <v>7.3117</v>
       </c>
       <c r="S2" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9911999702453613</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9896000027656555</v>
       </c>
       <c r="U2" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9896000027656555</v>
       </c>
     </row>
     <row r="3">
@@ -547,13 +547,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.005</v>
+        <v>0.0001</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F3" t="n">
         <v>200</v>
@@ -570,40 +570,40 @@
         <v>100</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0001</v>
+        <v>0.005</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9937000274658203</v>
       </c>
       <c r="M3" t="n">
-        <v>0.933899998664856</v>
+        <v>0.9853000044822693</v>
       </c>
       <c r="N3" t="n">
-        <v>113.91</v>
+        <v>100.529</v>
       </c>
       <c r="O3" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="P3" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0098</v>
       </c>
       <c r="Q3" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="R3" t="n">
-        <v>5.6955</v>
+        <v>7.733</v>
       </c>
       <c r="S3" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9918000102043152</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9915000200271606</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9915000200271606</v>
       </c>
     </row>
     <row r="4">
@@ -616,13 +616,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.005</v>
+        <v>0.0001</v>
       </c>
       <c r="D4" t="n">
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F4" t="n">
         <v>200</v>
@@ -639,40 +639,40 @@
         <v>100</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0001</v>
+        <v>0.005</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9926999807357788</v>
       </c>
       <c r="M4" t="n">
-        <v>0.933899998664856</v>
+        <v>0.9824000000953674</v>
       </c>
       <c r="N4" t="n">
-        <v>113.91</v>
+        <v>87.73999999999999</v>
       </c>
       <c r="O4" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0113</v>
       </c>
       <c r="P4" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0112</v>
       </c>
       <c r="Q4" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="R4" t="n">
-        <v>5.6955</v>
+        <v>7.3117</v>
       </c>
       <c r="S4" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9911999702453613</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9896000027656555</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9896000027656555</v>
       </c>
     </row>
     <row r="5">
@@ -685,13 +685,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.005</v>
+        <v>0.0001</v>
       </c>
       <c r="D5" t="n">
         <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F5" t="n">
         <v>200</v>
@@ -708,40 +708,40 @@
         <v>100</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0001</v>
+        <v>0.005</v>
       </c>
       <c r="K5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9937000274658203</v>
       </c>
       <c r="M5" t="n">
-        <v>0.933899998664856</v>
+        <v>0.9853000044822693</v>
       </c>
       <c r="N5" t="n">
-        <v>113.91</v>
+        <v>100.529</v>
       </c>
       <c r="O5" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="P5" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0098</v>
       </c>
       <c r="Q5" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="R5" t="n">
-        <v>5.6955</v>
+        <v>7.733</v>
       </c>
       <c r="S5" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9918000102043152</v>
       </c>
       <c r="T5" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9915000200271606</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9915000200271606</v>
       </c>
     </row>
     <row r="6">
@@ -754,13 +754,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.005</v>
+        <v>0.0001</v>
       </c>
       <c r="D6" t="n">
         <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F6" t="n">
         <v>200</v>
@@ -777,40 +777,40 @@
         <v>100</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0001</v>
+        <v>0.005</v>
       </c>
       <c r="K6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L6" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9926999807357788</v>
       </c>
       <c r="M6" t="n">
-        <v>0.933899998664856</v>
+        <v>0.9824000000953674</v>
       </c>
       <c r="N6" t="n">
-        <v>113.91</v>
+        <v>87.73999999999999</v>
       </c>
       <c r="O6" t="n">
-        <v>0.008500000000000001</v>
+        <v>0.0113</v>
       </c>
       <c r="P6" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0112</v>
       </c>
       <c r="Q6" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="R6" t="n">
-        <v>5.6955</v>
+        <v>7.3117</v>
       </c>
       <c r="S6" t="n">
-        <v>0.967199981212616</v>
+        <v>0.9911999702453613</v>
       </c>
       <c r="T6" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9896000027656555</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9656000137329102</v>
+        <v>0.9896000027656555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>